<commit_message>
Calling template from API
</commit_message>
<xml_diff>
--- a/sbnz-integracija-projekta/kjar/src/main/resources/templatetable/patient_risk_cutoff.xlsx
+++ b/sbnz-integracija-projekta/kjar/src/main/resources/templatetable/patient_risk_cutoff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danic\Documents\8_semestar\SBNZ\anesthesiology_expert_system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danic\Documents\8_semestar\SBNZ\anesthesiology_expert_system\sbnz-integracija-projekta\kjar\src\main\resources\templatetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BBC034-0B76-44D3-91E0-CCF2DD72D0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68392B8-62CA-477D-BBFF-8B702F9BFE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{06B14730-D739-42BC-860E-16AFB038C429}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8964" xr2:uid="{06B14730-D739-42BC-860E-16AFB038C429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
-    <t>HIGH</t>
-  </si>
-  <si>
     <t>ageLower</t>
   </si>
   <si>
@@ -46,6 +37,15 @@
   </si>
   <si>
     <t>risk</t>
+  </si>
+  <si>
+    <t>Patient.PatientRisk.MEDIUM</t>
+  </si>
+  <si>
+    <t>Patient.PatientRisk.HIGH</t>
+  </si>
+  <si>
+    <t>Patient.PatientRisk.LOW</t>
   </si>
 </sst>
 </file>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E510BF7E-EE4C-4B9B-B230-F6BAE1B13358}">
   <dimension ref="F6:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,16 +425,16 @@
   <sheetData>
     <row r="6" spans="6:9" x14ac:dyDescent="0.3">
       <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="6:9" x14ac:dyDescent="0.3">
@@ -448,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="6:9" x14ac:dyDescent="0.3">
@@ -462,7 +462,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="6:9" x14ac:dyDescent="0.3">
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="6:9" x14ac:dyDescent="0.3">
@@ -490,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="6:9" x14ac:dyDescent="0.3">
@@ -504,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="6:9" x14ac:dyDescent="0.3">
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="6:9" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="6:9" x14ac:dyDescent="0.3">
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="6:9" x14ac:dyDescent="0.3">
@@ -560,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="6:9" x14ac:dyDescent="0.3">
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>